<commit_message>
Homework and final exam
</commit_message>
<xml_diff>
--- a/StatsAssignment#4/DJIASP500.xlsx
+++ b/StatsAssignment#4/DJIASP500.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Trevorcardoza/Documents/GitHub/Statistics/StatsAssignment#4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4872C5-7D01-3B40-885C-DA3F30142E9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C3EB07-C30C-6A42-8480-107EC03E566A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="0" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v2.0" hidden="1">Data!$A$2:$A$16</definedName>
@@ -27,7 +28,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -44,6 +47,81 @@
   </si>
   <si>
     <t>S&amp;P</t>
+  </si>
+  <si>
+    <t>SUMMARY OUTPUT</t>
+  </si>
+  <si>
+    <t>Regression Statistics</t>
+  </si>
+  <si>
+    <t>Multiple R</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>Adjusted R Square</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Significance F</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Lower 95%</t>
+  </si>
+  <si>
+    <t>Upper 95%</t>
+  </si>
+  <si>
+    <t>Lower 95.0%</t>
+  </si>
+  <si>
+    <t>Upper 95.0%</t>
+  </si>
+  <si>
+    <t>X Variable 1</t>
   </si>
 </sst>
 </file>
@@ -53,7 +131,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -67,6 +145,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -76,7 +161,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -84,17 +169,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -179,8 +292,38 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1394,11 +1537,237 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CA5BB9-39B2-3D47-99A1-D436EAB79C45}">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.97395805184789919</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.94859428675935509</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.94464000112545932</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="4">
+        <v>9.6081058452101509</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4">
+        <v>22145.629260207432</v>
+      </c>
+      <c r="D12" s="4">
+        <v>22145.629260207432</v>
+      </c>
+      <c r="E12" s="4">
+        <v>239.89017855161859</v>
+      </c>
+      <c r="F12" s="4">
+        <v>9.2918358395624979E-10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4">
+        <v>13</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1200.1040731258988</v>
+      </c>
+      <c r="D13" s="4">
+        <v>92.315697932761452</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5">
+        <v>14</v>
+      </c>
+      <c r="C14" s="5">
+        <v>23345.73333333333</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="4">
+        <v>-669.02123824647447</v>
+      </c>
+      <c r="C17" s="4">
+        <v>130.73358151180096</v>
+      </c>
+      <c r="D17" s="4">
+        <v>-5.1174398384097186</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1.9761095642329129E-4</v>
+      </c>
+      <c r="F17" s="4">
+        <v>-951.4539700916929</v>
+      </c>
+      <c r="G17" s="4">
+        <v>-386.58850640125604</v>
+      </c>
+      <c r="H17" s="4">
+        <v>-951.4539700916929</v>
+      </c>
+      <c r="I17" s="4">
+        <v>-386.58850640125604</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0.15726702317885133</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1.0153866111067751E-2</v>
+      </c>
+      <c r="D18" s="5">
+        <v>15.488388507253379</v>
+      </c>
+      <c r="E18" s="5">
+        <v>9.2918358395624979E-10</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.13533092909058081</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0.17920311726712185</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0.13533092909058081</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0.17920311726712185</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="B2" sqref="B2:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>